<commit_message>
update to phpexcell support for php 7
</commit_message>
<xml_diff>
--- a/application/views/rpt/ru/doc/nakladnaya.xlsx
+++ b/application/views/rpt/ru/doc/nakladnaya.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\wamp\www\isell3\application\views\rpt\ru\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="360" yWindow="30" windowWidth="7455" windowHeight="6240"/>
   </bookViews>
@@ -436,7 +431,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -470,6 +464,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -742,7 +737,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1153,223 +1148,223 @@
       <c r="B15" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
-      <c r="I15" s="22"/>
-      <c r="J15" s="22"/>
-      <c r="K15" s="22" t="s">
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="21"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="L15" s="22"/>
-      <c r="M15" s="22"/>
-      <c r="N15" s="22"/>
-      <c r="O15" s="23" t="s">
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="P15" s="23"/>
-      <c r="Q15" s="23"/>
-      <c r="R15" s="24" t="s">
+      <c r="P15" s="22"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="S15" s="24"/>
-      <c r="T15" s="24"/>
-      <c r="U15" s="25" t="s">
+      <c r="S15" s="23"/>
+      <c r="T15" s="23"/>
+      <c r="U15" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="V15" s="25"/>
-      <c r="W15" s="25"/>
-      <c r="X15" s="25"/>
+      <c r="V15" s="24"/>
+      <c r="W15" s="24"/>
+      <c r="X15" s="24"/>
       <c r="Y15" s="7" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="16" spans="2:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K16" s="26" t="s">
+      <c r="K16" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="L16" s="26"/>
-      <c r="M16" s="26"/>
-      <c r="N16" s="26"/>
-      <c r="O16" s="26"/>
-      <c r="P16" s="26"/>
-      <c r="Q16" s="26"/>
-      <c r="R16" s="26"/>
-      <c r="S16" s="26"/>
-      <c r="T16" s="26"/>
-      <c r="U16" s="26"/>
-      <c r="V16" s="26"/>
-      <c r="W16" s="26"/>
-      <c r="X16" s="26"/>
+      <c r="L16" s="25"/>
+      <c r="M16" s="25"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="25"/>
+      <c r="P16" s="25"/>
+      <c r="Q16" s="25"/>
+      <c r="R16" s="25"/>
+      <c r="S16" s="25"/>
+      <c r="T16" s="25"/>
+      <c r="U16" s="25"/>
+      <c r="V16" s="25"/>
+      <c r="W16" s="25"/>
+      <c r="X16" s="25"/>
       <c r="Y16" s="8" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K17" s="26" t="s">
+      <c r="K17" s="25" t="s">
         <v>54</v>
       </c>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="26"/>
-      <c r="P17" s="26"/>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="26"/>
-      <c r="S17" s="26"/>
-      <c r="T17" s="26"/>
-      <c r="U17" s="26"/>
-      <c r="V17" s="26"/>
-      <c r="W17" s="26"/>
-      <c r="X17" s="26"/>
+      <c r="L17" s="25"/>
+      <c r="M17" s="25"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="25"/>
+      <c r="P17" s="25"/>
+      <c r="Q17" s="25"/>
+      <c r="R17" s="25"/>
+      <c r="S17" s="25"/>
+      <c r="T17" s="25"/>
+      <c r="U17" s="25"/>
+      <c r="V17" s="25"/>
+      <c r="W17" s="25"/>
+      <c r="X17" s="25"/>
       <c r="Y17" s="8" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="K18" s="26" t="s">
+      <c r="K18" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
-      <c r="N18" s="26"/>
-      <c r="O18" s="26"/>
-      <c r="P18" s="26"/>
-      <c r="Q18" s="26"/>
-      <c r="R18" s="26"/>
-      <c r="S18" s="26"/>
-      <c r="T18" s="26"/>
-      <c r="U18" s="26"/>
-      <c r="V18" s="26"/>
-      <c r="W18" s="26"/>
-      <c r="X18" s="26"/>
+      <c r="L18" s="25"/>
+      <c r="M18" s="25"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="25"/>
+      <c r="P18" s="25"/>
+      <c r="Q18" s="25"/>
+      <c r="R18" s="25"/>
+      <c r="S18" s="25"/>
+      <c r="T18" s="25"/>
+      <c r="U18" s="25"/>
+      <c r="V18" s="25"/>
+      <c r="W18" s="25"/>
+      <c r="X18" s="25"/>
       <c r="Y18" s="8" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="20" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="27"/>
-      <c r="Q20" s="27"/>
-      <c r="R20" s="27"/>
-      <c r="S20" s="27"/>
-      <c r="T20" s="27"/>
-      <c r="U20" s="27"/>
-      <c r="V20" s="27"/>
-      <c r="W20" s="27"/>
-      <c r="X20" s="27"/>
-      <c r="Y20" s="27"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="26"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="J20" s="26"/>
+      <c r="K20" s="26"/>
+      <c r="L20" s="26"/>
+      <c r="M20" s="26"/>
+      <c r="N20" s="26"/>
+      <c r="O20" s="26"/>
+      <c r="P20" s="26"/>
+      <c r="Q20" s="26"/>
+      <c r="R20" s="26"/>
+      <c r="S20" s="26"/>
+      <c r="T20" s="26"/>
+      <c r="U20" s="26"/>
+      <c r="V20" s="26"/>
+      <c r="W20" s="26"/>
+      <c r="X20" s="26"/>
+      <c r="Y20" s="26"/>
     </row>
     <row r="21" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="20" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="21"/>
-      <c r="M21" s="21"/>
-      <c r="N21" s="21"/>
-      <c r="O21" s="21"/>
-      <c r="P21" s="21"/>
-      <c r="Q21" s="21"/>
-      <c r="R21" s="21"/>
-      <c r="S21" s="21"/>
-      <c r="T21" s="21"/>
-      <c r="U21" s="21"/>
-      <c r="V21" s="21"/>
-      <c r="W21" s="21"/>
-      <c r="X21" s="21"/>
-      <c r="Y21" s="21"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
+      <c r="G21" s="20"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="20"/>
+      <c r="J21" s="20"/>
+      <c r="K21" s="20"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="20"/>
+      <c r="Q21" s="20"/>
+      <c r="R21" s="20"/>
+      <c r="S21" s="20"/>
+      <c r="T21" s="20"/>
+      <c r="U21" s="20"/>
+      <c r="V21" s="20"/>
+      <c r="W21" s="20"/>
+      <c r="X21" s="20"/>
+      <c r="Y21" s="20"/>
     </row>
     <row r="22" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="23" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="29"/>
-      <c r="C23" s="29"/>
-      <c r="D23" s="29"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="I23" s="18" t="s">
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="I23" s="29" t="s">
         <v>49</v>
       </c>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="29" t="s">
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
+      <c r="L23" s="29"/>
+      <c r="M23" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="N23" s="29"/>
-      <c r="O23" s="29"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="18"/>
-      <c r="R23" s="18"/>
-      <c r="S23" s="18"/>
-      <c r="T23" s="18"/>
-      <c r="U23" s="18"/>
-      <c r="V23" s="18"/>
-      <c r="X23" s="18"/>
-      <c r="Y23" s="18"/>
+      <c r="N23" s="28"/>
+      <c r="O23" s="28"/>
+      <c r="P23" s="29"/>
+      <c r="Q23" s="29"/>
+      <c r="R23" s="29"/>
+      <c r="S23" s="29"/>
+      <c r="T23" s="29"/>
+      <c r="U23" s="29"/>
+      <c r="V23" s="29"/>
+      <c r="X23" s="29"/>
+      <c r="Y23" s="29"/>
     </row>
     <row r="24" spans="1:25" ht="14.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E24" s="28" t="s">
+      <c r="E24" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="28"/>
-      <c r="G24" s="28"/>
-      <c r="I24" s="28" t="s">
+      <c r="F24" s="27"/>
+      <c r="G24" s="27"/>
+      <c r="I24" s="27" t="s">
         <v>28</v>
       </c>
-      <c r="J24" s="28"/>
-      <c r="K24" s="28"/>
-      <c r="L24" s="28"/>
-      <c r="P24" s="28" t="s">
+      <c r="J24" s="27"/>
+      <c r="K24" s="27"/>
+      <c r="L24" s="27"/>
+      <c r="P24" s="27" t="s">
         <v>29</v>
       </c>
-      <c r="Q24" s="28"/>
-      <c r="R24" s="28"/>
-      <c r="S24" s="28"/>
-      <c r="T24" s="28"/>
-      <c r="U24" s="28"/>
-      <c r="V24" s="28"/>
-      <c r="X24" s="19" t="s">
+      <c r="Q24" s="27"/>
+      <c r="R24" s="27"/>
+      <c r="S24" s="27"/>
+      <c r="T24" s="27"/>
+      <c r="U24" s="27"/>
+      <c r="V24" s="27"/>
+      <c r="X24" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="Y24" s="19"/>
+      <c r="Y24" s="18"/>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="X25" s="20"/>
-      <c r="Y25" s="20"/>
+      <c r="X25" s="19"/>
+      <c r="Y25" s="19"/>
     </row>
     <row r="26" spans="1:25" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B26" s="11" t="s">
@@ -1401,7 +1396,6 @@
     </row>
   </sheetData>
   <mergeCells count="50">
-    <mergeCell ref="M23:O23"/>
     <mergeCell ref="E23:G23"/>
     <mergeCell ref="I23:L23"/>
     <mergeCell ref="P23:V23"/>
@@ -1421,6 +1415,7 @@
     <mergeCell ref="I24:L24"/>
     <mergeCell ref="P24:V24"/>
     <mergeCell ref="A23:D23"/>
+    <mergeCell ref="M23:O23"/>
     <mergeCell ref="G9:Y9"/>
     <mergeCell ref="B10:F10"/>
     <mergeCell ref="G10:Y10"/>
@@ -1452,8 +1447,8 @@
     <mergeCell ref="G8:Y8"/>
     <mergeCell ref="B9:F9"/>
   </mergeCells>
-  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="90" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="90" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>